<commit_message>
finishing up the data dictionary
</commit_message>
<xml_diff>
--- a/dasc2103project_DataDictionary.xlsx
+++ b/dasc2103project_DataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobhaarala/Dropbox/My Mac (Jacob’s MacBook Air)/Downloads/Data-Structures&amp;Algorithms/dasc2103project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DE0B3C-7A03-474E-9C41-0F7BEC881514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642A8942-1962-634E-9177-3FA1EBBDC5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15320" windowHeight="16460" xr2:uid="{94DDB44B-70C4-0A46-A739-5D6D65E68943}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13240" windowHeight="16460" xr2:uid="{94DDB44B-70C4-0A46-A739-5D6D65E68943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="85">
   <si>
     <t>Header</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>75th percentile of earnings but only undergraduate</t>
+  </si>
+  <si>
+    <t>The increase in average wages that graduate students can expect having earned a degree from a graduate program</t>
+  </si>
+  <si>
+    <t>Graduate students as a share of the total</t>
   </si>
 </sst>
 </file>
@@ -644,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C70223C-A419-9C48-8A4D-6A96E48F12A8}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1205,6 +1211,9 @@
       <c r="A40" t="s">
         <v>40</v>
       </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
       <c r="C40" t="s">
         <v>43</v>
       </c>
@@ -1215,6 +1224,9 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>83</v>
       </c>
       <c r="C41" t="s">
         <v>43</v>

</xml_diff>